<commit_message>
Last minute changes to the LP functionality
Also, edited the excel sheet to have 1 more sheet for the user to manually key in the calls for the doctors for the last 2 days of the previous schedule month
</commit_message>
<xml_diff>
--- a/information_excel.xlsx
+++ b/information_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ttsh-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD5508B-B542-41C2-94B8-4955F4A212E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECDD3DF-0ED1-4976-9E03-FD781CA17DD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Training" sheetId="1" r:id="rId3"/>
     <sheet name="Priority Leave" sheetId="3" r:id="rId4"/>
     <sheet name="Public Holiday" sheetId="4" r:id="rId5"/>
+    <sheet name="Last 2 Days Calls" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="213">
   <si>
     <t>Email</t>
   </si>
@@ -675,6 +676,9 @@
   </si>
   <si>
     <t>ASB</t>
+  </si>
+  <si>
+    <t>Duty Date</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402572E3-A301-453A-BBD2-7FEA71DA364E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2921,4 +2925,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8EA2D1-C746-4C78-8899-F0CFEE569256}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="15">
+        <v>43889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15">
+        <v>43889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="15">
+        <v>43890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="15">
+        <v>43890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="15">
+        <v>43890</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>